<commit_message>
clarify infected population size
</commit_message>
<xml_diff>
--- a/variant_sampling_workbook.xlsx
+++ b/variant_sampling_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirleewohl/Desktop/Lessler-Lab/github/epiphyanies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirleewohl/Desktop/Lessler-Lab/github/VOCsamplesize/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D334970C-4EE4-A149-8217-3BC6BAB9CF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBFD7BC-15A2-B048-8BF0-FB6A32E5B00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="2020" windowWidth="27540" windowHeight="19160" xr2:uid="{82711159-A3A1-6543-B722-8D858F78A64C}"/>
+    <workbookView xWindow="4940" yWindow="2020" windowWidth="27540" windowHeight="19160" activeTab="5" xr2:uid="{82711159-A3A1-6543-B722-8D858F78A64C}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="123">
   <si>
     <t>Desired probability of detection:</t>
   </si>
@@ -466,13 +466,7 @@
     <t>Number of variant introductions</t>
   </si>
   <si>
-    <t>Population size</t>
-  </si>
-  <si>
     <t>Growth rate (per time step)</t>
-  </si>
-  <si>
-    <t>the population size of the geographic region in which sampling is to be conducted</t>
   </si>
   <si>
     <r>
@@ -1041,6 +1035,15 @@
   </si>
   <si>
     <t>Determine confidence in estimate of variant prevalence: cross-sectional sample</t>
+  </si>
+  <si>
+    <t>Infected population size</t>
+  </si>
+  <si>
+    <t>the total number of infections in the geographic region in which sampling is to be conducted (at the time when the variant is introduced)</t>
+  </si>
+  <si>
+    <t>Infected population size:</t>
   </si>
 </sst>
 </file>
@@ -1331,9 +1334,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1350,6 +1350,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1666,7 +1669,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4748040A-BC4E-FF45-AF4B-9454F8204D7F}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1700,22 +1705,22 @@
     </row>
     <row r="2" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19"/>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
       <c r="P2" s="19"/>
       <c r="Q2" s="19"/>
       <c r="R2" s="19"/>
@@ -1742,213 +1747,213 @@
     </row>
     <row r="4" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
-      <c r="B4" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
+      <c r="B4" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
       <c r="P4" s="19"/>
       <c r="Q4" s="19"/>
       <c r="R4" s="19"/>
     </row>
     <row r="5" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
     </row>
     <row r="6" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+    </row>
+    <row r="7" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D7" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+    </row>
+    <row r="8" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-    </row>
-    <row r="7" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28" t="s">
+      <c r="D8" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+    </row>
+    <row r="9" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D9" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
-    </row>
-    <row r="8" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28" t="s">
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+    </row>
+    <row r="10" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-    </row>
-    <row r="9" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="28" t="s">
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+    </row>
+    <row r="11" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-    </row>
-    <row r="10" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" s="28" t="s">
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+    </row>
+    <row r="12" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-    </row>
-    <row r="11" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-    </row>
-    <row r="12" spans="1:18" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
     </row>
     <row r="13" spans="1:18" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
@@ -1972,22 +1977,22 @@
     </row>
     <row r="14" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
-      <c r="B14" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
+      <c r="B14" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
       <c r="P14" s="19"/>
       <c r="Q14" s="19"/>
       <c r="R14" s="19"/>
@@ -2120,13 +2125,13 @@
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
@@ -2224,7 +2229,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -2244,13 +2249,13 @@
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="24" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>60</v>
+        <v>121</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
@@ -2270,13 +2275,13 @@
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" s="25">
         <v>0.1</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -2342,13 +2347,13 @@
       <c r="A29" s="19"/>
       <c r="B29" s="19"/>
       <c r="C29" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="25" t="s">
-        <v>64</v>
-      </c>
       <c r="E29" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
@@ -2368,13 +2373,13 @@
       <c r="A30" s="19"/>
       <c r="B30" s="19"/>
       <c r="C30" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D30" s="26">
         <v>0.8</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
@@ -2440,13 +2445,13 @@
       <c r="A33" s="19"/>
       <c r="B33" s="19"/>
       <c r="C33" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D33" s="25">
         <v>0.05</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
@@ -2466,13 +2471,13 @@
       <c r="A34" s="19"/>
       <c r="B34" s="19"/>
       <c r="C34" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D34" s="26">
         <v>0.3</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
@@ -2578,13 +2583,13 @@
       <c r="A39" s="19"/>
       <c r="B39" s="19"/>
       <c r="C39" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D39" s="25">
         <v>0.25</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
@@ -2604,13 +2609,13 @@
       <c r="A40" s="19"/>
       <c r="B40" s="19"/>
       <c r="C40" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D40" s="26">
         <v>0.97499999999999998</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
@@ -2630,13 +2635,13 @@
       <c r="A41" s="19"/>
       <c r="B41" s="19"/>
       <c r="C41" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D41" s="25">
         <v>0.8</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
@@ -2700,13 +2705,13 @@
       <c r="A44" s="19"/>
       <c r="B44" s="19"/>
       <c r="C44" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D44" s="25">
         <v>0.4</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
@@ -2726,13 +2731,13 @@
       <c r="A45" s="19"/>
       <c r="B45" s="19"/>
       <c r="C45" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D45" s="26">
         <v>0.95</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
@@ -2752,13 +2757,13 @@
       <c r="A46" s="19"/>
       <c r="B46" s="19"/>
       <c r="C46" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D46" s="25">
         <v>0.6</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
@@ -2796,22 +2801,22 @@
     </row>
     <row r="48" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="19"/>
-      <c r="B48" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32"/>
-      <c r="N48" s="32"/>
-      <c r="O48" s="32"/>
+      <c r="B48" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="31"/>
+      <c r="O48" s="31"/>
       <c r="P48" s="19"/>
       <c r="Q48" s="19"/>
       <c r="R48" s="19"/>
@@ -2885,7 +2890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4E9E52-3664-524A-876D-099CF82F6C22}">
   <dimension ref="B1:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2905,23 +2910,23 @@
     <row r="1" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="F4" s="27" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="F4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3012,7 +3017,7 @@
         <v>0.8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -3145,8 +3150,8 @@
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="33" t="s">
-        <v>108</v>
+      <c r="B33" s="32" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3182,23 +3187,23 @@
     <row r="1" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="F4" s="27" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="F4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3219,7 +3224,7 @@
     </row>
     <row r="7" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="10">
         <v>100</v>
@@ -3241,7 +3246,7 @@
         <v>0.02</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G8" s="10">
         <f>ROUNDUP(C7*C12,0)</f>
@@ -3261,7 +3266,7 @@
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
       <c r="F10" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G10" s="13">
         <f>ROUND(1-(1-G7)^G8,2)</f>
@@ -3277,7 +3282,7 @@
         <v>30</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H11" s="3"/>
     </row>
@@ -3289,7 +3294,7 @@
         <v>0.8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -3422,8 +3427,8 @@
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="33" t="s">
-        <v>108</v>
+      <c r="B33" s="32" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3459,23 +3464,23 @@
     <row r="1" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="F4" s="27" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="F4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3582,7 +3587,7 @@
         <v>0.8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H13" s="3"/>
     </row>
@@ -3715,8 +3720,8 @@
       </c>
     </row>
     <row r="34" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="33" t="s">
-        <v>108</v>
+      <c r="B34" s="32" t="s">
+        <v>106</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="3"/>
@@ -3757,23 +3762,23 @@
     <row r="1" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="F4" s="27" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="F4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3794,7 +3799,7 @@
     </row>
     <row r="7" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="10">
         <v>200</v>
@@ -3816,7 +3821,7 @@
         <v>0.1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G8" s="10">
         <f>C7*C13</f>
@@ -3832,7 +3837,7 @@
         <v>0.25</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G9" s="10">
         <f>ROUND(SQRT((G8*((G7*C9)^2))/(G7*(1-G7))),2)</f>
@@ -3852,7 +3857,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
       <c r="F11" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G11" s="13">
         <f>ROUND(1-(2*(1-_xlfn.NORM.S.DIST(G9,TRUE))),2)</f>
@@ -3868,7 +3873,7 @@
         <v>30</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -3880,7 +3885,7 @@
         <v>0.8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H13" s="3"/>
     </row>
@@ -4013,8 +4018,8 @@
       </c>
     </row>
     <row r="34" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="33" t="s">
-        <v>108</v>
+      <c r="B34" s="32" t="s">
+        <v>106</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="3"/>
@@ -4035,8 +4040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2078EFDD-813E-BD4C-9CAA-EE77C2EA4E46}">
   <dimension ref="B1:H40"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4055,23 +4060,23 @@
     <row r="1" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="F4" s="27" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="F4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4092,7 +4097,7 @@
     </row>
     <row r="7" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -4130,10 +4135,10 @@
     </row>
     <row r="10" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>30</v>
@@ -4162,7 +4167,7 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="F12" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G12" s="10">
         <f>IF(C10&lt;&gt;"NA",ROUND(1/(1+(G10*EXP(-C15*C10))),3),ROUND(C9/(C9+(G6*(1-C9))),3))</f>
@@ -4181,7 +4186,7 @@
     </row>
     <row r="14" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>122</v>
       </c>
       <c r="C14" s="10">
         <v>10000</v>
@@ -4262,7 +4267,7 @@
     <row r="20" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="11"/>
       <c r="F20" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H20" s="8"/>
     </row>
@@ -4273,7 +4278,7 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="F21" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H21" s="3"/>
     </row>
@@ -4400,8 +4405,8 @@
       <c r="H38" s="1"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="33" t="s">
-        <v>108</v>
+      <c r="B40" s="32" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -4437,23 +4442,23 @@
     <row r="1" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="F4" s="27" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="F4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4474,13 +4479,13 @@
     </row>
     <row r="7" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" s="10">
         <v>20</v>
@@ -4512,10 +4517,10 @@
     </row>
     <row r="10" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>30</v>
@@ -4544,7 +4549,7 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="F12" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G12" s="10">
         <f>IF(C10&lt;&gt;"NA",ROUND(1/(1+(G10*EXP(-C15*C10))),3),ROUND(C9/(C9+(G6*(1-C9))),3))</f>
@@ -4617,7 +4622,7 @@
         <v>30</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G18" s="10">
         <f>ROUNDDOWN(C8*C19,0)</f>
@@ -4637,7 +4642,7 @@
     <row r="20" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="11"/>
       <c r="F20" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G20" s="13">
         <f>ROUND(1-EXP(-1*G18*G16),2)</f>
@@ -4652,7 +4657,7 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="F21" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H21" s="3"/>
     </row>
@@ -4663,7 +4668,7 @@
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="F22" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H22" s="3"/>
     </row>
@@ -4782,8 +4787,8 @@
       <c r="H38" s="1"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="33" t="s">
-        <v>108</v>
+      <c r="B40" s="32" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix rounding errors in periodic detection calculation
</commit_message>
<xml_diff>
--- a/variant_sampling_workbook.xlsx
+++ b/variant_sampling_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swohl/Desktop/work/github/VOCsamplesize/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E9289E-4FEE-7940-8D64-8C8287173B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFC18E6-AF2D-0847-8774-DCCA30A4346D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="27540" windowHeight="19160" xr2:uid="{82711159-A3A1-6543-B722-8D858F78A64C}"/>
+    <workbookView xWindow="4980" yWindow="1740" windowWidth="29400" windowHeight="21800" activeTab="5" xr2:uid="{82711159-A3A1-6543-B722-8D858F78A64C}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -1375,7 +1375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1442,9 +1442,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1453,6 +1450,12 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1770,7 +1773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4748040A-BC4E-FF45-AF4B-9454F8204D7F}">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
@@ -1828,22 +1831,22 @@
     </row>
     <row r="3" spans="1:18" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16"/>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
       <c r="P3" s="16"/>
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
@@ -3112,16 +3115,16 @@
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="F4" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3336,7 +3339,7 @@
   <dimension ref="B1:H33"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3362,16 +3365,16 @@
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="F4" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3431,7 +3434,7 @@
       <c r="F10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="28">
         <f>1-(1-G7)^G8</f>
         <v>0.88958719163513256</v>
       </c>
@@ -3586,7 +3589,7 @@
   <dimension ref="B1:H34"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3612,16 +3615,16 @@
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="F4" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3882,16 +3885,16 @@
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="F4" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3966,7 +3969,7 @@
       <c r="F11" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="28">
         <f>1-(2*(1-_xlfn.NORM.S.DIST(G9,TRUE)))</f>
         <v>0.74985612872569951</v>
       </c>
@@ -4125,8 +4128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2078EFDD-813E-BD4C-9CAA-EE77C2EA4E46}">
   <dimension ref="B1:H40"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4152,16 +4155,16 @@
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="F4" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4175,8 +4178,7 @@
         <v>130</v>
       </c>
       <c r="G6" s="7">
-        <f>(C29*C30*((C28*C23)+((1-C28)*C24)))/(C35*C36*((C34*C23)+((1-C34)*C24)))</f>
-        <v>1.3684210526315792</v>
+        <v>1.0589999999999999</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -4190,14 +4192,14 @@
         <v>0</v>
       </c>
       <c r="C8" s="8">
-        <v>0.95</v>
+        <v>0.75</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G8" s="8">
         <f>C13/C14</f>
-        <v>2.9999999999999997E-4</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4212,7 +4214,7 @@
       </c>
       <c r="G9" s="7">
         <f>(1/G8)-1</f>
-        <v>3332.3333333333335</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4227,7 +4229,7 @@
       </c>
       <c r="G10" s="7">
         <f>(1/G6)*((1/G8)-1)</f>
-        <v>2435.1666666666661</v>
+        <v>9441.9263456090666</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4236,7 +4238,7 @@
       </c>
       <c r="G11" s="8">
         <f>IF(C9&lt;&gt;"NA",ROUNDUP(-(1/C15)*LN((1/G9)*((1/C9)-1)),0),"NA")</f>
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4250,7 +4252,7 @@
       </c>
       <c r="G12" s="8">
         <f>IF(C10&lt;&gt;"NA",ROUND(1/(1+(G10*EXP(-C15*C10))),3),ROUND(C9/(C9+((1/G6)*(1-C9))),3))</f>
-        <v>1.4E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4258,7 +4260,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4273,7 +4275,7 @@
       </c>
       <c r="G14" s="7">
         <f>IF(C9&lt;&gt;"NA",(1/C15)*LN(G10+EXP(C15*G11)),(1/C15)*LN(G10+EXP(C15*C10)))</f>
-        <v>78.126877093260148</v>
+        <v>91.644925941357101</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4288,7 +4290,7 @@
       </c>
       <c r="G15" s="7">
         <f>(1/C15)*LN(G10+EXP(C15*0))</f>
-        <v>77.981810446612371</v>
+        <v>91.530212053395076</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4297,7 +4299,7 @@
       </c>
       <c r="G16" s="7">
         <f>G14-G15</f>
-        <v>0.14506664664777702</v>
+        <v>0.11471388796202575</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4318,9 +4320,9 @@
       <c r="F18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="8">
-        <f>ROUNDUP(-LN(1-C8)/G16,0)</f>
-        <v>21</v>
+      <c r="G18" s="29">
+        <f>(-LN(1-C8)/G16)</f>
+        <v>12.084799719967663</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4335,7 +4337,7 @@
       </c>
       <c r="G19" s="10">
         <f>ROUNDUP(G18/C19,0)</f>
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4481,7 +4483,7 @@
   <dimension ref="B1:H40"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4507,16 +4509,16 @@
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="F4" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4690,7 +4692,7 @@
       <c r="F20" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="28">
         <f>1-EXP(-1*G18*G16)</f>
         <v>0.901831152223042</v>
       </c>

</xml_diff>

<commit_message>
fix cod calculation typo
</commit_message>
<xml_diff>
--- a/variant_sampling_workbook.xlsx
+++ b/variant_sampling_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swohl/Desktop/work/github/VOCsamplesize/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFC18E6-AF2D-0847-8774-DCCA30A4346D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0D65D0-BDF0-604A-A787-6DE716588CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="1740" windowWidth="29400" windowHeight="21800" activeTab="5" xr2:uid="{82711159-A3A1-6543-B722-8D858F78A64C}"/>
+    <workbookView xWindow="7320" yWindow="500" windowWidth="29400" windowHeight="21800" activeTab="5" xr2:uid="{82711159-A3A1-6543-B722-8D858F78A64C}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -3859,7 +3859,7 @@
   <dimension ref="B1:H34"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4129,7 +4129,7 @@
   <dimension ref="B1:H40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4178,7 +4178,8 @@
         <v>130</v>
       </c>
       <c r="G6" s="7">
-        <v>1.0589999999999999</v>
+        <f>(C29*C30*((C28*C23)+((1-C28)*C24)))/(C35*C36*((C34*C23)+((1-C34)*C24)))</f>
+        <v>1.3684210526315792</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -4192,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="8">
-        <v>0.75</v>
+        <v>0.95</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>28</v>
@@ -4229,7 +4230,7 @@
       </c>
       <c r="G10" s="7">
         <f>(1/G6)*((1/G8)-1)</f>
-        <v>9441.9263456090666</v>
+        <v>7306.9615384615372</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4252,7 +4253,7 @@
       </c>
       <c r="G12" s="8">
         <f>IF(C10&lt;&gt;"NA",ROUND(1/(1+(G10*EXP(-C15*C10))),3),ROUND(C9/(C9+((1/G6)*(1-C9))),3))</f>
-        <v>1.0999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4275,7 +4276,7 @@
       </c>
       <c r="G14" s="7">
         <f>IF(C9&lt;&gt;"NA",(1/C15)*LN(G10+EXP(C15*G11)),(1/C15)*LN(G10+EXP(C15*C10)))</f>
-        <v>91.644925941357101</v>
+        <v>89.115176335731292</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4290,7 +4291,7 @@
       </c>
       <c r="G15" s="7">
         <f>(1/C15)*LN(G10+EXP(C15*0))</f>
-        <v>91.530212053395076</v>
+        <v>88.967196545477506</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4299,7 +4300,7 @@
       </c>
       <c r="G16" s="7">
         <f>G14-G15</f>
-        <v>0.11471388796202575</v>
+        <v>0.14797979025378538</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4322,7 +4323,7 @@
       </c>
       <c r="G18" s="29">
         <f>(-LN(1-C8)/G16)</f>
-        <v>12.084799719967663</v>
+        <v>20.244198673456072</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4337,7 +4338,7 @@
       </c>
       <c r="G19" s="10">
         <f>ROUNDUP(G18/C19,0)</f>
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4440,7 +4441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>4</v>
       </c>
@@ -4448,7 +4449,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
@@ -4483,7 +4484,7 @@
   <dimension ref="B1:H40"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4795,7 +4796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>4</v>
       </c>
@@ -4803,7 +4804,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>